<commit_message>
[added] Project v2 tested and decode happens in 2nd cycle
</commit_message>
<xml_diff>
--- a/Project-v1/Documents/Memory/NO_haza_no_forw_WRONG/no_haza_no_forw_WRONG_MEM.xlsx
+++ b/Project-v1/Documents/Memory/NO_haza_no_forw_WRONG/no_haza_no_forw_WRONG_MEM.xlsx
@@ -214,22 +214,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +536,7 @@
   <dimension ref="A1:AW22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH17" sqref="AH17"/>
+      <selection activeCell="AH22" sqref="AH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,26 +546,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" t="s">
         <v>1</v>
       </c>
@@ -595,11 +595,11 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
       <c r="H3" t="s">
         <v>1</v>
       </c>
@@ -624,11 +624,11 @@
       <c r="U3" s="10"/>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
       <c r="I4" t="s">
         <v>1</v>
       </c>
@@ -652,11 +652,11 @@
       <c r="V4" s="10"/>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
       <c r="J5" s="4" t="s">
         <v>1</v>
       </c>
@@ -707,11 +707,11 @@
       <c r="AQ5" s="4"/>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
@@ -741,13 +741,13 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
-      <c r="V6" s="14" t="s">
+      <c r="V6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
@@ -766,16 +766,16 @@
       <c r="AW6" s="10"/>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="11" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
@@ -802,17 +802,17 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
-      <c r="X7" s="14" t="s">
+      <c r="X7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
@@ -835,11 +835,11 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -892,14 +892,14 @@
       <c r="AW8" s="10"/>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="11" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -955,11 +955,11 @@
       <c r="AW9" s="10"/>
     </row>
     <row r="10" spans="1:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="13" t="s">
         <v>27</v>
       </c>
@@ -999,34 +999,34 @@
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
-      <c r="AD10" s="14" t="s">
+      <c r="AD10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
-      <c r="AG10" s="14"/>
-      <c r="AH10" s="14"/>
-      <c r="AI10" s="14"/>
-      <c r="AJ10" s="14"/>
-      <c r="AK10" s="14"/>
-      <c r="AL10" s="14"/>
-      <c r="AM10" s="14"/>
-      <c r="AN10" s="14"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
       <c r="AO10" s="4"/>
       <c r="AP10" s="4"/>
       <c r="AQ10" s="4"/>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="11" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1063,19 +1063,19 @@
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
-      <c r="AE11" s="14" t="s">
+      <c r="AE11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="14"/>
-      <c r="AJ11" s="14"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
-      <c r="AN11" s="14"/>
-      <c r="AO11" s="14"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
       <c r="AP11" s="4"/>
       <c r="AQ11" s="4"/>
     </row>
@@ -1083,11 +1083,11 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -1148,11 +1148,11 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1209,12 +1209,12 @@
       <c r="AT13" s="10"/>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -1252,45 +1252,61 @@
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="8"/>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="AD10:AN10"/>
-    <mergeCell ref="AB9:AH9"/>
-    <mergeCell ref="AE11:AO11"/>
-    <mergeCell ref="AG12:AR12"/>
-    <mergeCell ref="AT8:AW8"/>
-    <mergeCell ref="AT9:AW9"/>
-    <mergeCell ref="Z8:AJ8"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="AI13:AT13"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D5:F5"/>
     <mergeCell ref="AT6:AW6"/>
     <mergeCell ref="X7:AF7"/>
     <mergeCell ref="AT7:AW7"/>
@@ -1302,29 +1318,13 @@
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="V6:Z6"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="AI13:AT13"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="AD10:AN10"/>
+    <mergeCell ref="AB9:AH9"/>
+    <mergeCell ref="AE11:AO11"/>
+    <mergeCell ref="AG12:AR12"/>
+    <mergeCell ref="AT8:AW8"/>
+    <mergeCell ref="AT9:AW9"/>
+    <mergeCell ref="Z8:AJ8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>